<commit_message>
Correct reference to Karsholt & Razowski
</commit_message>
<xml_diff>
--- a/CountryDistributions.xlsx
+++ b/CountryDistributions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\NetBeans Projects\pterophoroidea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A5AF8708-0E98-4057-98A3-E3D2F46D5A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2F4F8E4A-C1AD-45C2-850C-3BBCEFFF52B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="720" windowWidth="30696" windowHeight="16560"/>
   </bookViews>
@@ -2368,8 +2368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="C252" sqref="C252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2516,6 +2516,9 @@
       <c r="B16" t="s">
         <v>31</v>
       </c>
+      <c r="C16">
+        <v>979</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -2575,6 +2578,9 @@
       <c r="B23" t="s">
         <v>45</v>
       </c>
+      <c r="C23">
+        <v>979</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -2864,6 +2870,9 @@
       <c r="B58" t="s">
         <v>115</v>
       </c>
+      <c r="C58">
+        <v>979</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
@@ -3014,6 +3023,9 @@
       <c r="B76" t="s">
         <v>151</v>
       </c>
+      <c r="C76">
+        <v>979</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
@@ -3070,6 +3082,9 @@
       <c r="B83" t="s">
         <v>165</v>
       </c>
+      <c r="C83">
+        <v>979</v>
+      </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
@@ -3268,6 +3283,9 @@
       <c r="B107" t="s">
         <v>212</v>
       </c>
+      <c r="C107">
+        <v>979</v>
+      </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
@@ -3292,6 +3310,9 @@
       <c r="B110" t="s">
         <v>218</v>
       </c>
+      <c r="C110">
+        <v>979</v>
+      </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
@@ -3444,6 +3465,9 @@
       <c r="B129" t="s">
         <v>256</v>
       </c>
+      <c r="C129">
+        <v>979</v>
+      </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
@@ -3452,6 +3476,9 @@
       <c r="B130" t="s">
         <v>258</v>
       </c>
+      <c r="C130">
+        <v>979</v>
+      </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
@@ -3519,6 +3546,9 @@
       <c r="B138" t="s">
         <v>274</v>
       </c>
+      <c r="C138">
+        <v>979</v>
+      </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
@@ -3568,7 +3598,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>287</v>
       </c>
@@ -3576,7 +3606,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>289</v>
       </c>
@@ -3584,7 +3614,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>291</v>
       </c>
@@ -3592,7 +3622,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>293</v>
       </c>
@@ -3600,7 +3630,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>295</v>
       </c>
@@ -3608,7 +3638,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>297</v>
       </c>
@@ -3616,7 +3646,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>299</v>
       </c>
@@ -3624,7 +3654,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>301</v>
       </c>
@@ -3632,7 +3662,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>303</v>
       </c>
@@ -3640,7 +3670,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>305</v>
       </c>
@@ -3648,7 +3678,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>307</v>
       </c>
@@ -3656,15 +3686,18 @@
         <v>308</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>309</v>
       </c>
       <c r="B156" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C156">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>311</v>
       </c>
@@ -3672,7 +3705,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>313</v>
       </c>
@@ -3680,7 +3713,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>315</v>
       </c>
@@ -3688,7 +3721,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>317</v>
       </c>
@@ -3827,7 +3860,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>351</v>
       </c>
@@ -3835,7 +3868,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>353</v>
       </c>
@@ -3843,15 +3876,18 @@
         <v>354</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>355</v>
       </c>
       <c r="B179" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C179">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>357</v>
       </c>
@@ -3859,7 +3895,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>359</v>
       </c>
@@ -3867,7 +3903,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>361</v>
       </c>
@@ -3875,7 +3911,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>363</v>
       </c>
@@ -3883,15 +3919,18 @@
         <v>364</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>365</v>
       </c>
       <c r="B184" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C184">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>367</v>
       </c>
@@ -3899,7 +3938,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>369</v>
       </c>
@@ -3907,7 +3946,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>371</v>
       </c>
@@ -3915,7 +3954,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>373</v>
       </c>
@@ -3923,7 +3962,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>375</v>
       </c>
@@ -3931,7 +3970,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>377</v>
       </c>
@@ -3939,7 +3978,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>379</v>
       </c>
@@ -3947,7 +3986,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>381</v>
       </c>
@@ -4053,6 +4092,9 @@
       <c r="B204" t="s">
         <v>406</v>
       </c>
+      <c r="C204">
+        <v>979</v>
+      </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
@@ -4176,6 +4218,9 @@
       <c r="B219" t="s">
         <v>436</v>
       </c>
+      <c r="C219">
+        <v>979</v>
+      </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
@@ -4330,6 +4375,9 @@
       </c>
       <c r="B238" t="s">
         <v>474</v>
+      </c>
+      <c r="C238">
+        <v>979</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Central Asia, Agdistis kazakhstanicus
</commit_message>
<xml_diff>
--- a/CountryDistributions.xlsx
+++ b/CountryDistributions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\NetBeans Projects\pterophoroidea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2F4F8E4A-C1AD-45C2-850C-3BBCEFFF52B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1AA822D2-DE2B-4877-8FDB-DA1E422FD3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="720" windowWidth="30696" windowHeight="16560"/>
+    <workbookView xWindow="24" yWindow="96" windowWidth="30696" windowHeight="16560"/>
   </bookViews>
   <sheets>
     <sheet name="region" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="503">
   <si>
     <t>ID</t>
   </si>
@@ -1526,6 +1526,9 @@
   </si>
   <si>
     <t>referenceID</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -2368,8 +2371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
-      <selection activeCell="C252" sqref="C252"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2468,6 +2471,9 @@
       <c r="B10" t="s">
         <v>19</v>
       </c>
+      <c r="C10" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -2612,6 +2618,9 @@
       </c>
       <c r="B27" t="s">
         <v>53</v>
+      </c>
+      <c r="C27">
+        <v>1945</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>